<commit_message>
llm: 2 model with 2 language on L4 gpu
</commit_message>
<xml_diff>
--- a/Ka-ChatBot_BenchMark.xlsx
+++ b/Ka-ChatBot_BenchMark.xlsx
@@ -822,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,6 +851,26 @@
           <t>sts_score</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>en_gemma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>en_qwen</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fa_gemma</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>fa_qwen</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -868,6 +888,16 @@
       <c r="D2" t="n">
         <v>0.8858654499053955</v>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -886,6 +916,18 @@
       <c r="D3" t="n">
         <v>0.8564716577529907</v>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -902,6 +944,18 @@
       <c r="D4" t="n">
         <v>0.8705127835273743</v>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -919,6 +973,16 @@
       <c r="D5" t="n">
         <v>0.8531449437141418</v>
       </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -936,6 +1000,16 @@
       <c r="D6" t="n">
         <v>0.8588141202926636</v>
       </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -953,6 +1027,16 @@
       <c r="D7" t="n">
         <v>0.8558281064033508</v>
       </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -969,6 +1053,18 @@
       <c r="D8" t="n">
         <v>0.8513281941413879</v>
       </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -986,6 +1082,18 @@
       <c r="D9" t="n">
         <v>0.8459639549255371</v>
       </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1003,6 +1111,18 @@
       <c r="D10" t="n">
         <v>0.8408076763153076</v>
       </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1020,6 +1140,18 @@
       <c r="D11" t="n">
         <v>0.8568130731582642</v>
       </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1036,6 +1168,18 @@
       <c r="D12" t="n">
         <v>0.8491228222846985</v>
       </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1052,6 +1196,18 @@
       <c r="D13" t="n">
         <v>0.8441330194473267</v>
       </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1069,6 +1225,16 @@
       <c r="D14" t="n">
         <v>0.8552259206771851</v>
       </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1085,6 +1251,18 @@
       <c r="D15" t="n">
         <v>0.8605915307998657</v>
       </c>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1102,6 +1280,18 @@
       <c r="D16" t="n">
         <v>0.8765230178833008</v>
       </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1118,6 +1308,18 @@
       <c r="D17" t="n">
         <v>0.8470735549926758</v>
       </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1134,6 +1336,18 @@
       <c r="D18" t="n">
         <v>0.8505915999412537</v>
       </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1151,6 +1365,18 @@
       <c r="D19" t="n">
         <v>0.8577365875244141</v>
       </c>
+      <c r="E19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1167,6 +1393,18 @@
       <c r="D20" t="n">
         <v>0.8546472787857056</v>
       </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1184,6 +1422,18 @@
       <c r="D21" t="n">
         <v>0.8362616300582886</v>
       </c>
+      <c r="E21" t="n">
+        <v>9</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>9</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1200,6 +1450,18 @@
       <c r="D22" t="n">
         <v>0.8664118647575378</v>
       </c>
+      <c r="E22" t="n">
+        <v>19</v>
+      </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1216,6 +1478,18 @@
       <c r="D23" t="n">
         <v>0.8655897378921509</v>
       </c>
+      <c r="E23" t="n">
+        <v>5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5</v>
+      </c>
+      <c r="H23" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1232,6 +1506,18 @@
       <c r="D24" t="n">
         <v>0.8484431505203247</v>
       </c>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>5</v>
+      </c>
+      <c r="G24" t="n">
+        <v>19</v>
+      </c>
+      <c r="H24" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1248,6 +1534,18 @@
       <c r="D25" t="n">
         <v>0.8587133288383484</v>
       </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" t="n">
+        <v>9</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1264,6 +1562,18 @@
       <c r="D26" t="n">
         <v>0.8609504699707031</v>
       </c>
+      <c r="E26" t="n">
+        <v>5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1281,6 +1591,18 @@
       <c r="D27" t="n">
         <v>0.8460131883621216</v>
       </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>9</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1297,6 +1619,18 @@
       <c r="D28" t="n">
         <v>0.8244483470916748</v>
       </c>
+      <c r="E28" t="n">
+        <v>9</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>9</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1313,6 +1647,18 @@
       <c r="D29" t="n">
         <v>0.8729507923126221</v>
       </c>
+      <c r="E29" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" t="n">
+        <v>7</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7</v>
+      </c>
+      <c r="H29" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1329,6 +1675,18 @@
       <c r="D30" t="n">
         <v>0.9073020815849304</v>
       </c>
+      <c r="E30" t="n">
+        <v>6</v>
+      </c>
+      <c r="F30" t="n">
+        <v>6</v>
+      </c>
+      <c r="G30" t="n">
+        <v>6</v>
+      </c>
+      <c r="H30" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1345,6 +1703,18 @@
       <c r="D31" t="n">
         <v>0.9073020815849304</v>
       </c>
+      <c r="E31" t="n">
+        <v>6</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" t="n">
+        <v>6</v>
+      </c>
+      <c r="H31" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1361,6 +1731,18 @@
       <c r="D32" t="n">
         <v>0.8547959327697754</v>
       </c>
+      <c r="E32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>6</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6</v>
+      </c>
+      <c r="H32" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1377,6 +1759,16 @@
       <c r="D33" t="n">
         <v>0.8543360829353333</v>
       </c>
+      <c r="E33" t="n">
+        <v>6</v>
+      </c>
+      <c r="F33" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" t="n">
+        <v>6</v>
+      </c>
+      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1394,6 +1786,18 @@
       <c r="D34" t="n">
         <v>0.8601416349411011</v>
       </c>
+      <c r="E34" t="n">
+        <v>13</v>
+      </c>
+      <c r="F34" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" t="n">
+        <v>9</v>
+      </c>
+      <c r="H34" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1409,6 +1813,18 @@
       </c>
       <c r="D35" t="n">
         <v>0.8514372706413269</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6</v>
+      </c>
+      <c r="H35" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1428,6 +1844,18 @@
       <c r="D36" t="n">
         <v>0.8613648414611816</v>
       </c>
+      <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="n">
+        <v>7</v>
+      </c>
+      <c r="G36" t="n">
+        <v>6</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1444,6 +1872,18 @@
       <c r="D37" t="n">
         <v>0.8755484819412231</v>
       </c>
+      <c r="E37" t="n">
+        <v>7</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="n">
+        <v>7</v>
+      </c>
+      <c r="H37" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1460,6 +1900,18 @@
       <c r="D38" t="n">
         <v>0.8493435382843018</v>
       </c>
+      <c r="E38" t="n">
+        <v>8</v>
+      </c>
+      <c r="F38" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" t="n">
+        <v>8</v>
+      </c>
+      <c r="H38" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1476,6 +1928,18 @@
       <c r="D39" t="n">
         <v>0.8181660175323486</v>
       </c>
+      <c r="E39" t="n">
+        <v>8</v>
+      </c>
+      <c r="F39" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" t="n">
+        <v>8</v>
+      </c>
+      <c r="H39" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1492,6 +1956,18 @@
       <c r="D40" t="n">
         <v>0.8666313886642456</v>
       </c>
+      <c r="E40" t="n">
+        <v>8</v>
+      </c>
+      <c r="F40" t="n">
+        <v>8</v>
+      </c>
+      <c r="G40" t="n">
+        <v>8</v>
+      </c>
+      <c r="H40" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1508,6 +1984,18 @@
       <c r="D41" t="n">
         <v>0.8585730791091919</v>
       </c>
+      <c r="E41" t="n">
+        <v>8</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8</v>
+      </c>
+      <c r="G41" t="n">
+        <v>8</v>
+      </c>
+      <c r="H41" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1524,6 +2012,18 @@
       <c r="D42" t="n">
         <v>0.8466288447380066</v>
       </c>
+      <c r="E42" t="n">
+        <v>8</v>
+      </c>
+      <c r="F42" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" t="n">
+        <v>8</v>
+      </c>
+      <c r="H42" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1539,6 +2039,18 @@
       </c>
       <c r="D43" t="n">
         <v>0.8392025828361511</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+      <c r="F43" t="n">
+        <v>8</v>
+      </c>
+      <c r="G43" t="n">
+        <v>8</v>
+      </c>
+      <c r="H43" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="44">
@@ -1558,6 +2070,18 @@
       <c r="D44" t="n">
         <v>0.8402473926544189</v>
       </c>
+      <c r="E44" t="n">
+        <v>8</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G44" t="n">
+        <v>8</v>
+      </c>
+      <c r="H44" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1574,6 +2098,18 @@
       <c r="D45" t="n">
         <v>0.8811037540435791</v>
       </c>
+      <c r="E45" t="n">
+        <v>9</v>
+      </c>
+      <c r="F45" t="n">
+        <v>9</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9</v>
+      </c>
+      <c r="H45" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1590,6 +2126,18 @@
       <c r="D46" t="n">
         <v>0.8946105241775513</v>
       </c>
+      <c r="E46" t="n">
+        <v>9</v>
+      </c>
+      <c r="F46" t="n">
+        <v>9</v>
+      </c>
+      <c r="G46" t="n">
+        <v>9</v>
+      </c>
+      <c r="H46" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1607,6 +2155,18 @@
       <c r="D47" t="n">
         <v>0.8416050672531128</v>
       </c>
+      <c r="E47" t="n">
+        <v>9</v>
+      </c>
+      <c r="F47" t="n">
+        <v>9</v>
+      </c>
+      <c r="G47" t="n">
+        <v>9</v>
+      </c>
+      <c r="H47" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1623,6 +2183,18 @@
       <c r="D48" t="n">
         <v>0.8340308666229248</v>
       </c>
+      <c r="E48" t="n">
+        <v>9</v>
+      </c>
+      <c r="F48" t="n">
+        <v>9</v>
+      </c>
+      <c r="G48" t="n">
+        <v>9</v>
+      </c>
+      <c r="H48" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1639,6 +2211,18 @@
       <c r="D49" t="n">
         <v>0.859331488609314</v>
       </c>
+      <c r="E49" t="n">
+        <v>9</v>
+      </c>
+      <c r="F49" t="n">
+        <v>9</v>
+      </c>
+      <c r="G49" t="n">
+        <v>9</v>
+      </c>
+      <c r="H49" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1656,6 +2240,18 @@
       <c r="D50" t="n">
         <v>0.8572762608528137</v>
       </c>
+      <c r="E50" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" t="n">
+        <v>10</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10</v>
+      </c>
+      <c r="H50" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1673,6 +2269,16 @@
       <c r="D51" t="n">
         <v>0.8617393970489502</v>
       </c>
+      <c r="E51" t="n">
+        <v>9</v>
+      </c>
+      <c r="F51" t="n">
+        <v>10</v>
+      </c>
+      <c r="G51" t="n">
+        <v>10</v>
+      </c>
+      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1689,6 +2295,18 @@
       <c r="D52" t="n">
         <v>0.8994492292404175</v>
       </c>
+      <c r="E52" t="n">
+        <v>10</v>
+      </c>
+      <c r="F52" t="n">
+        <v>10</v>
+      </c>
+      <c r="G52" t="n">
+        <v>10</v>
+      </c>
+      <c r="H52" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1705,6 +2323,18 @@
       <c r="D53" t="n">
         <v>0.8859749436378479</v>
       </c>
+      <c r="E53" t="n">
+        <v>10</v>
+      </c>
+      <c r="F53" t="n">
+        <v>10</v>
+      </c>
+      <c r="G53" t="n">
+        <v>10</v>
+      </c>
+      <c r="H53" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1721,6 +2351,18 @@
       <c r="D54" t="n">
         <v>0.882864236831665</v>
       </c>
+      <c r="E54" t="n">
+        <v>10</v>
+      </c>
+      <c r="F54" t="n">
+        <v>10</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10</v>
+      </c>
+      <c r="H54" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1738,6 +2380,16 @@
       <c r="D55" t="n">
         <v>0.8481650948524475</v>
       </c>
+      <c r="E55" t="n">
+        <v>11</v>
+      </c>
+      <c r="F55" t="n">
+        <v>10</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11</v>
+      </c>
+      <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1754,6 +2406,16 @@
       <c r="D56" t="n">
         <v>0.8641391396522522</v>
       </c>
+      <c r="E56" t="n">
+        <v>11</v>
+      </c>
+      <c r="F56" t="n">
+        <v>12</v>
+      </c>
+      <c r="G56" t="n">
+        <v>10</v>
+      </c>
+      <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1770,6 +2432,18 @@
       <c r="D57" t="n">
         <v>0.8448090553283691</v>
       </c>
+      <c r="E57" t="n">
+        <v>11</v>
+      </c>
+      <c r="F57" t="n">
+        <v>11</v>
+      </c>
+      <c r="G57" t="n">
+        <v>11</v>
+      </c>
+      <c r="H57" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1785,6 +2459,18 @@
       </c>
       <c r="D58" t="n">
         <v>0.8479213714599609</v>
+      </c>
+      <c r="E58" t="n">
+        <v>11</v>
+      </c>
+      <c r="F58" t="n">
+        <v>16</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11</v>
+      </c>
+      <c r="H58" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="59">
@@ -1804,6 +2490,18 @@
       <c r="D59" t="n">
         <v>0.8545359969139099</v>
       </c>
+      <c r="E59" t="n">
+        <v>11</v>
+      </c>
+      <c r="F59" t="n">
+        <v>11</v>
+      </c>
+      <c r="G59" t="n">
+        <v>11</v>
+      </c>
+      <c r="H59" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1819,6 +2517,18 @@
       </c>
       <c r="D60" t="n">
         <v>0.8433393836021423</v>
+      </c>
+      <c r="E60" t="n">
+        <v>11</v>
+      </c>
+      <c r="F60" t="n">
+        <v>11</v>
+      </c>
+      <c r="G60" t="n">
+        <v>10</v>
+      </c>
+      <c r="H60" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="61">
@@ -1839,6 +2549,16 @@
       <c r="D61" t="n">
         <v>0.8529068231582642</v>
       </c>
+      <c r="E61" t="n">
+        <v>11</v>
+      </c>
+      <c r="F61" t="n">
+        <v>11</v>
+      </c>
+      <c r="G61" t="n">
+        <v>11</v>
+      </c>
+      <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1855,6 +2575,18 @@
       <c r="D62" t="n">
         <v>0.8766939640045166</v>
       </c>
+      <c r="E62" t="n">
+        <v>11</v>
+      </c>
+      <c r="F62" t="n">
+        <v>11</v>
+      </c>
+      <c r="G62" t="n">
+        <v>11</v>
+      </c>
+      <c r="H62" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1871,6 +2603,18 @@
       <c r="D63" t="n">
         <v>0.8381291627883911</v>
       </c>
+      <c r="E63" t="n">
+        <v>12</v>
+      </c>
+      <c r="F63" t="n">
+        <v>11</v>
+      </c>
+      <c r="G63" t="n">
+        <v>12</v>
+      </c>
+      <c r="H63" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1887,6 +2631,18 @@
       <c r="D64" t="n">
         <v>0.8507808446884155</v>
       </c>
+      <c r="E64" t="n">
+        <v>13</v>
+      </c>
+      <c r="F64" t="n">
+        <v>9</v>
+      </c>
+      <c r="G64" t="n">
+        <v>13</v>
+      </c>
+      <c r="H64" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1903,6 +2659,18 @@
       <c r="D65" t="n">
         <v>0.809970498085022</v>
       </c>
+      <c r="E65" t="n">
+        <v>13</v>
+      </c>
+      <c r="F65" t="n">
+        <v>13</v>
+      </c>
+      <c r="G65" t="n">
+        <v>13</v>
+      </c>
+      <c r="H65" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1919,6 +2687,18 @@
       <c r="D66" t="n">
         <v>0.8801558017730713</v>
       </c>
+      <c r="E66" t="n">
+        <v>14</v>
+      </c>
+      <c r="F66" t="n">
+        <v>14</v>
+      </c>
+      <c r="G66" t="n">
+        <v>9</v>
+      </c>
+      <c r="H66" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1935,6 +2715,18 @@
       <c r="D67" t="n">
         <v>0.8643205165863037</v>
       </c>
+      <c r="E67" t="n">
+        <v>14</v>
+      </c>
+      <c r="F67" t="n">
+        <v>14</v>
+      </c>
+      <c r="G67" t="n">
+        <v>9</v>
+      </c>
+      <c r="H67" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1951,6 +2743,18 @@
       <c r="D68" t="n">
         <v>0.8706686496734619</v>
       </c>
+      <c r="E68" t="n">
+        <v>13</v>
+      </c>
+      <c r="F68" t="n">
+        <v>14</v>
+      </c>
+      <c r="G68" t="n">
+        <v>13</v>
+      </c>
+      <c r="H68" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1968,6 +2772,18 @@
       <c r="D69" t="n">
         <v>0.8521902561187744</v>
       </c>
+      <c r="E69" t="n">
+        <v>13</v>
+      </c>
+      <c r="F69" t="n">
+        <v>9</v>
+      </c>
+      <c r="G69" t="n">
+        <v>13</v>
+      </c>
+      <c r="H69" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1984,6 +2800,18 @@
       <c r="D70" t="n">
         <v>0.8788481950759888</v>
       </c>
+      <c r="E70" t="n">
+        <v>13</v>
+      </c>
+      <c r="F70" t="n">
+        <v>14</v>
+      </c>
+      <c r="G70" t="n">
+        <v>13</v>
+      </c>
+      <c r="H70" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2001,6 +2829,18 @@
       <c r="D71" t="n">
         <v>0.8304421901702881</v>
       </c>
+      <c r="E71" t="n">
+        <v>20</v>
+      </c>
+      <c r="F71" t="n">
+        <v>16</v>
+      </c>
+      <c r="G71" t="n">
+        <v>5</v>
+      </c>
+      <c r="H71" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2018,6 +2858,18 @@
       <c r="D72" t="n">
         <v>0.8542701005935669</v>
       </c>
+      <c r="E72" t="n">
+        <v>17</v>
+      </c>
+      <c r="F72" t="n">
+        <v>16</v>
+      </c>
+      <c r="G72" t="n">
+        <v>17</v>
+      </c>
+      <c r="H72" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2034,6 +2886,18 @@
       <c r="D73" t="n">
         <v>0.8525227904319763</v>
       </c>
+      <c r="E73" t="n">
+        <v>16</v>
+      </c>
+      <c r="F73" t="n">
+        <v>16</v>
+      </c>
+      <c r="G73" t="n">
+        <v>9</v>
+      </c>
+      <c r="H73" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2050,6 +2914,18 @@
       <c r="D74" t="n">
         <v>0.9245259761810303</v>
       </c>
+      <c r="E74" t="n">
+        <v>17</v>
+      </c>
+      <c r="F74" t="n">
+        <v>17</v>
+      </c>
+      <c r="G74" t="n">
+        <v>17</v>
+      </c>
+      <c r="H74" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2066,6 +2942,18 @@
       </c>
       <c r="D75" t="n">
         <v>0.8431832790374756</v>
+      </c>
+      <c r="E75" t="n">
+        <v>17</v>
+      </c>
+      <c r="F75" t="n">
+        <v>18</v>
+      </c>
+      <c r="G75" t="n">
+        <v>17</v>
+      </c>
+      <c r="H75" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="76">
@@ -2085,6 +2973,18 @@
       <c r="D76" t="n">
         <v>0.849095344543457</v>
       </c>
+      <c r="E76" t="n">
+        <v>18</v>
+      </c>
+      <c r="F76" t="n">
+        <v>18</v>
+      </c>
+      <c r="G76" t="n">
+        <v>18</v>
+      </c>
+      <c r="H76" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2101,6 +3001,18 @@
       <c r="D77" t="n">
         <v>0.8673208951950073</v>
       </c>
+      <c r="E77" t="n">
+        <v>19</v>
+      </c>
+      <c r="F77" t="n">
+        <v>19</v>
+      </c>
+      <c r="G77" t="n">
+        <v>20</v>
+      </c>
+      <c r="H77" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2118,6 +3030,18 @@
       <c r="D78" t="n">
         <v>0.8824416399002075</v>
       </c>
+      <c r="E78" t="n">
+        <v>19</v>
+      </c>
+      <c r="F78" t="n">
+        <v>19</v>
+      </c>
+      <c r="G78" t="n">
+        <v>19</v>
+      </c>
+      <c r="H78" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2135,6 +3059,18 @@
       <c r="D79" t="n">
         <v>0.8717066645622253</v>
       </c>
+      <c r="E79" t="n">
+        <v>20</v>
+      </c>
+      <c r="F79" t="n">
+        <v>20</v>
+      </c>
+      <c r="G79" t="n">
+        <v>20</v>
+      </c>
+      <c r="H79" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2151,6 +3087,18 @@
       <c r="D80" t="n">
         <v>0.879250168800354</v>
       </c>
+      <c r="E80" t="n">
+        <v>20</v>
+      </c>
+      <c r="F80" t="n">
+        <v>20</v>
+      </c>
+      <c r="G80" t="n">
+        <v>20</v>
+      </c>
+      <c r="H80" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2166,6 +3114,18 @@
       </c>
       <c r="D81" t="n">
         <v>0.9020805358886719</v>
+      </c>
+      <c r="E81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F81" t="n">
+        <v>20</v>
+      </c>
+      <c r="G81" t="n">
+        <v>20</v>
+      </c>
+      <c r="H81" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="82">
@@ -2185,6 +3145,18 @@
       <c r="D82" t="n">
         <v>0.8386732935905457</v>
       </c>
+      <c r="E82" t="n">
+        <v>21</v>
+      </c>
+      <c r="F82" t="n">
+        <v>21</v>
+      </c>
+      <c r="G82" t="n">
+        <v>21</v>
+      </c>
+      <c r="H82" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2201,6 +3173,18 @@
       <c r="D83" t="n">
         <v>0.851478636264801</v>
       </c>
+      <c r="E83" t="n">
+        <v>21</v>
+      </c>
+      <c r="F83" t="n">
+        <v>21</v>
+      </c>
+      <c r="G83" t="n">
+        <v>21</v>
+      </c>
+      <c r="H83" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2217,6 +3201,18 @@
       <c r="D84" t="n">
         <v>0.839668333530426</v>
       </c>
+      <c r="E84" t="n">
+        <v>21</v>
+      </c>
+      <c r="F84" t="n">
+        <v>21</v>
+      </c>
+      <c r="G84" t="n">
+        <v>21</v>
+      </c>
+      <c r="H84" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2233,6 +3229,18 @@
       <c r="D85" t="n">
         <v>0.8655587434768677</v>
       </c>
+      <c r="E85" t="n">
+        <v>21</v>
+      </c>
+      <c r="F85" t="n">
+        <v>21</v>
+      </c>
+      <c r="G85" t="n">
+        <v>21</v>
+      </c>
+      <c r="H85" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2250,6 +3258,18 @@
       <c r="D86" t="n">
         <v>0.8576963543891907</v>
       </c>
+      <c r="E86" t="n">
+        <v>21</v>
+      </c>
+      <c r="F86" t="n">
+        <v>21</v>
+      </c>
+      <c r="G86" t="n">
+        <v>21</v>
+      </c>
+      <c r="H86" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2266,6 +3286,18 @@
       <c r="D87" t="n">
         <v>0.8727791309356689</v>
       </c>
+      <c r="E87" t="n">
+        <v>21</v>
+      </c>
+      <c r="F87" t="n">
+        <v>21</v>
+      </c>
+      <c r="G87" t="n">
+        <v>21</v>
+      </c>
+      <c r="H87" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2282,6 +3314,18 @@
       </c>
       <c r="D88" t="n">
         <v>0.8650441765785217</v>
+      </c>
+      <c r="E88" t="n">
+        <v>21</v>
+      </c>
+      <c r="F88" t="n">
+        <v>21</v>
+      </c>
+      <c r="G88" t="n">
+        <v>21</v>
+      </c>
+      <c r="H88" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="89">
@@ -2301,6 +3345,18 @@
       <c r="D89" t="n">
         <v>0.8503273129463196</v>
       </c>
+      <c r="E89" t="n">
+        <v>22</v>
+      </c>
+      <c r="F89" t="n">
+        <v>22</v>
+      </c>
+      <c r="G89" t="n">
+        <v>22</v>
+      </c>
+      <c r="H89" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2316,6 +3372,18 @@
       </c>
       <c r="D90" t="n">
         <v>0.8679998517036438</v>
+      </c>
+      <c r="E90" t="n">
+        <v>22</v>
+      </c>
+      <c r="F90" t="n">
+        <v>22</v>
+      </c>
+      <c r="G90" t="n">
+        <v>22</v>
+      </c>
+      <c r="H90" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="91">
@@ -2335,6 +3403,18 @@
       <c r="D91" t="n">
         <v>0.8222296833992004</v>
       </c>
+      <c r="E91" t="n">
+        <v>23</v>
+      </c>
+      <c r="F91" t="n">
+        <v>23</v>
+      </c>
+      <c r="G91" t="n">
+        <v>23</v>
+      </c>
+      <c r="H91" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2351,6 +3431,18 @@
       </c>
       <c r="D92" t="n">
         <v>0.8910433053970337</v>
+      </c>
+      <c r="E92" t="n">
+        <v>23</v>
+      </c>
+      <c r="F92" t="n">
+        <v>23</v>
+      </c>
+      <c r="G92" t="n">
+        <v>23</v>
+      </c>
+      <c r="H92" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="93">
@@ -2370,6 +3462,18 @@
       <c r="D93" t="n">
         <v>0.8735889196395874</v>
       </c>
+      <c r="E93" t="n">
+        <v>23</v>
+      </c>
+      <c r="F93" t="n">
+        <v>23</v>
+      </c>
+      <c r="G93" t="n">
+        <v>23</v>
+      </c>
+      <c r="H93" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2385,6 +3489,18 @@
       </c>
       <c r="D94" t="n">
         <v>0.8605258464813232</v>
+      </c>
+      <c r="E94" t="n">
+        <v>14</v>
+      </c>
+      <c r="F94" t="n">
+        <v>24</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>